<commit_message>
Unit Value Uzerine  Calısmalar
</commit_message>
<xml_diff>
--- a/Data_Sources_and_Preparation/Explanation of Data and Sources.xlsx
+++ b/Data_Sources_and_Preparation/Explanation of Data and Sources.xlsx
@@ -616,8 +616,8 @@
       <xdr:rowOff>7117</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>444032</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1247596</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>94563</xdr:rowOff>
     </xdr:to>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A33" zoomScale="110" zoomScaleNormal="90" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="110" zoomScaleNormal="90" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -923,7 +923,7 @@
     <col min="1" max="2" width="23.5546875" customWidth="1"/>
     <col min="3" max="3" width="36.33203125" customWidth="1"/>
     <col min="4" max="4" width="40.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
     <col min="6" max="8" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Data range revised to 1 to 8 months
</commit_message>
<xml_diff>
--- a/Data_Sources_and_Preparation/Explanation of Data and Sources.xlsx
+++ b/Data_Sources_and_Preparation/Explanation of Data and Sources.xlsx
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="223">
   <si>
     <t xml:space="preserve">Economic Policy Uncertainty </t>
   </si>
@@ -787,6 +787,9 @@
   </si>
   <si>
     <t>VARIABLE FOR CHINA</t>
+  </si>
+  <si>
+    <t>PPI Icin kullanılan tablo</t>
   </si>
 </sst>
 </file>
@@ -1466,6 +1469,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>283657</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>75352</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2142067" y="12810067"/>
+          <a:ext cx="8276190" cy="6780952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1732,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2837,6 +2878,11 @@
       </c>
       <c r="C44" s="13"/>
       <c r="E44" s="13"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>222</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K31"/>

</xml_diff>